<commit_message>
modify: add table for Grid Search only
</commit_message>
<xml_diff>
--- a/2020_01_32770/Result.xlsx
+++ b/2020_01_32770/Result.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Random Search</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -8181,7 +8181,7 @@
         <v>0.10054950999999999</v>
       </c>
       <c r="H33" s="5">
-        <f t="shared" ref="H33:Q42" si="1">INDEX($C$4:$C$124, (ROW()-33)*11+(COLUMN()-7)+1)</f>
+        <f t="shared" ref="H33:Q43" si="1">INDEX($C$4:$C$124, (ROW()-33)*11+(COLUMN()-7)+1)</f>
         <v>6.2419589999999997E-2</v>
       </c>
       <c r="I33" s="5">
@@ -8236,7 +8236,7 @@
         <v>6.1594099999999997E-3</v>
       </c>
       <c r="G34" s="5">
-        <f t="shared" ref="G34:Q42" si="3">INDEX($C$4:$C$124, (ROW()-33)*11+(COLUMN()-7)+1)</f>
+        <f t="shared" ref="G34:Q43" si="3">INDEX($C$4:$C$124, (ROW()-33)*11+(COLUMN()-7)+1)</f>
         <v>1.0613E-4</v>
       </c>
       <c r="H34" s="5">
@@ -8762,6 +8762,54 @@
       <c r="C43">
         <v>3.7534700000000001E-3</v>
       </c>
+      <c r="F43" s="4">
+        <f t="shared" ref="F43" si="4">INDEX(A$4:A$124, (ROW()-32)*11)</f>
+        <v>6.1594110000000001E-2</v>
+      </c>
+      <c r="G43" s="5">
+        <f t="shared" si="3"/>
+        <v>2.1043E-4</v>
+      </c>
+      <c r="H43" s="5">
+        <f t="shared" si="1"/>
+        <v>6.0574999999999995E-4</v>
+      </c>
+      <c r="I43" s="5">
+        <f t="shared" si="1"/>
+        <v>1.75427E-3</v>
+      </c>
+      <c r="J43" s="5">
+        <f t="shared" si="1"/>
+        <v>3.11671E-3</v>
+      </c>
+      <c r="K43" s="5">
+        <f t="shared" si="1"/>
+        <v>1.51906E-3</v>
+      </c>
+      <c r="L43" s="5">
+        <f t="shared" si="1"/>
+        <v>6.2578399999999998E-3</v>
+      </c>
+      <c r="M43" s="5">
+        <f t="shared" si="1"/>
+        <v>2.68768E-3</v>
+      </c>
+      <c r="N43" s="5">
+        <f t="shared" si="1"/>
+        <v>3.1391100000000001E-3</v>
+      </c>
+      <c r="O43" s="5">
+        <f t="shared" si="1"/>
+        <v>5.2181600000000003E-3</v>
+      </c>
+      <c r="P43" s="5">
+        <f t="shared" si="1"/>
+        <v>9.3728100000000005E-3</v>
+      </c>
+      <c r="Q43" s="5">
+        <f t="shared" si="1"/>
+        <v>9.8893799999999997E-3</v>
+      </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A44">
@@ -9668,6 +9716,20 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="G33:Q42">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="2.5000000000000001E-2"/>
+        <color theme="3" tint="0.39997558519241921"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{56B47B0C-2F22-4B5B-B815-191346AA218E}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G43:Q43">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9676,7 +9738,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{56B47B0C-2F22-4B5B-B815-191346AA218E}</x14:id>
+          <x14:id>{3271B2A7-7398-4942-BFA0-4102DDD67412}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9705,6 +9767,21 @@
           </x14:cfRule>
           <xm:sqref>G33:Q42</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{3271B2A7-7398-4942-BFA0-4102DDD67412}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2.5000000000000001E-2</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G43:Q43</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>
@@ -9713,13 +9790,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C125"/>
+  <dimension ref="A1:Q125"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="6" max="17" width="10.25" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
@@ -9879,7 +9959,7 @@
         <v>1.18139E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -9890,7 +9970,7 @@
         <v>1.7269399999999999E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -9901,7 +9981,7 @@
         <v>6.7297800000000003E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -9912,7 +9992,7 @@
         <v>2.8408299999999999E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -9923,7 +10003,7 @@
         <v>3.004882E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -9934,7 +10014,7 @@
         <v>8.1275400000000008E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -9945,7 +10025,7 @@
         <v>8.7766100000000007E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -9956,7 +10036,7 @@
         <v>1.310152E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -9967,7 +10047,7 @@
         <v>1.2520140000000001E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -9978,7 +10058,7 @@
         <v>1.297338E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>0.05</v>
       </c>
@@ -9989,7 +10069,7 @@
         <v>1.4980000000000001E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>0.05</v>
       </c>
@@ -10000,7 +10080,7 @@
         <v>6.4526699999999998E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>0.05</v>
       </c>
@@ -10011,7 +10091,7 @@
         <v>2.0390199999999999E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>0.05</v>
       </c>
@@ -10022,7 +10102,7 @@
         <v>5.6041199999999998E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>0.05</v>
       </c>
@@ -10033,7 +10113,7 @@
         <v>4.2066899999999999E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>0.05</v>
       </c>
@@ -10044,7 +10124,7 @@
         <v>1.1602070000000001E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>0.05</v>
       </c>
@@ -10054,8 +10134,55 @@
       <c r="C32">
         <v>1.5081209999999999E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F32" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" s="4">
+        <f>INDEX($B4:$B14, COLUMN()-6)</f>
+        <v>0</v>
+      </c>
+      <c r="H32" s="4">
+        <f t="shared" ref="H32:Q32" si="0">INDEX($B4:$B14, COLUMN()-6)</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="I32" s="4">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="J32" s="4">
+        <f t="shared" si="0"/>
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="K32" s="4">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="L32" s="4">
+        <f t="shared" si="0"/>
+        <v>0.375</v>
+      </c>
+      <c r="M32" s="4">
+        <f t="shared" si="0"/>
+        <v>0.45</v>
+      </c>
+      <c r="N32" s="4">
+        <f t="shared" si="0"/>
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="O32" s="4">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="P32" s="4">
+        <f t="shared" si="0"/>
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="Q32" s="4">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>0.05</v>
       </c>
@@ -10065,8 +10192,56 @@
       <c r="C33">
         <v>1.2655410000000001E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F33" s="4">
+        <f>INDEX(A$4:A$124, (ROW()-32)*11)</f>
+        <v>0</v>
+      </c>
+      <c r="G33" s="5">
+        <f>INDEX($C$4:$C$124, (ROW()-33)*11+(COLUMN()-7)+1)</f>
+        <v>7.0891040000000002E-2</v>
+      </c>
+      <c r="H33" s="5">
+        <f t="shared" ref="H33:Q43" si="1">INDEX($C$4:$C$124, (ROW()-33)*11+(COLUMN()-7)+1)</f>
+        <v>5.6976730000000003E-2</v>
+      </c>
+      <c r="I33" s="5">
+        <f t="shared" si="1"/>
+        <v>6.3149510000000006E-2</v>
+      </c>
+      <c r="J33" s="5">
+        <f t="shared" si="1"/>
+        <v>5.644859E-2</v>
+      </c>
+      <c r="K33" s="5">
+        <f t="shared" si="1"/>
+        <v>5.674481E-2</v>
+      </c>
+      <c r="L33" s="5">
+        <f t="shared" si="1"/>
+        <v>7.5658970000000006E-2</v>
+      </c>
+      <c r="M33" s="5">
+        <f t="shared" si="1"/>
+        <v>5.1133970000000001E-2</v>
+      </c>
+      <c r="N33" s="5">
+        <f t="shared" si="1"/>
+        <v>8.8448020000000002E-2</v>
+      </c>
+      <c r="O33" s="5">
+        <f t="shared" si="1"/>
+        <v>0.10847683</v>
+      </c>
+      <c r="P33" s="5">
+        <f t="shared" si="1"/>
+        <v>7.5442640000000005E-2</v>
+      </c>
+      <c r="Q33" s="5">
+        <f t="shared" si="1"/>
+        <v>9.6383570000000002E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>0.05</v>
       </c>
@@ -10076,8 +10251,56 @@
       <c r="C34">
         <v>3.0585709999999999E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F34" s="4">
+        <f t="shared" ref="F34:F43" si="2">INDEX(A$4:A$124, (ROW()-32)*11)</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G34" s="5">
+        <f t="shared" ref="G34:Q43" si="3">INDEX($C$4:$C$124, (ROW()-33)*11+(COLUMN()-7)+1)</f>
+        <v>1.2011E-4</v>
+      </c>
+      <c r="H34" s="5">
+        <f t="shared" si="1"/>
+        <v>1.18139E-3</v>
+      </c>
+      <c r="I34" s="5">
+        <f t="shared" si="1"/>
+        <v>1.7269399999999999E-3</v>
+      </c>
+      <c r="J34" s="5">
+        <f t="shared" si="1"/>
+        <v>6.7297800000000003E-3</v>
+      </c>
+      <c r="K34" s="5">
+        <f t="shared" si="1"/>
+        <v>2.8408299999999999E-3</v>
+      </c>
+      <c r="L34" s="5">
+        <f t="shared" si="1"/>
+        <v>3.004882E-2</v>
+      </c>
+      <c r="M34" s="5">
+        <f t="shared" si="1"/>
+        <v>8.1275400000000008E-3</v>
+      </c>
+      <c r="N34" s="5">
+        <f t="shared" si="1"/>
+        <v>8.7766100000000007E-3</v>
+      </c>
+      <c r="O34" s="5">
+        <f t="shared" si="1"/>
+        <v>1.310152E-2</v>
+      </c>
+      <c r="P34" s="5">
+        <f t="shared" si="1"/>
+        <v>1.2520140000000001E-2</v>
+      </c>
+      <c r="Q34" s="5">
+        <f t="shared" si="1"/>
+        <v>1.297338E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>0.05</v>
       </c>
@@ -10087,8 +10310,56 @@
       <c r="C35">
         <v>1.7063689999999999E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F35" s="4">
+        <f t="shared" si="2"/>
+        <v>0.05</v>
+      </c>
+      <c r="G35" s="5">
+        <f t="shared" si="3"/>
+        <v>1.4980000000000001E-4</v>
+      </c>
+      <c r="H35" s="5">
+        <f t="shared" si="1"/>
+        <v>6.4526699999999998E-3</v>
+      </c>
+      <c r="I35" s="5">
+        <f t="shared" si="1"/>
+        <v>2.0390199999999999E-3</v>
+      </c>
+      <c r="J35" s="5">
+        <f t="shared" si="1"/>
+        <v>5.6041199999999998E-3</v>
+      </c>
+      <c r="K35" s="5">
+        <f t="shared" si="1"/>
+        <v>4.2066899999999999E-3</v>
+      </c>
+      <c r="L35" s="5">
+        <f t="shared" si="1"/>
+        <v>1.1602070000000001E-2</v>
+      </c>
+      <c r="M35" s="5">
+        <f t="shared" si="1"/>
+        <v>1.5081209999999999E-2</v>
+      </c>
+      <c r="N35" s="5">
+        <f t="shared" si="1"/>
+        <v>1.2655410000000001E-2</v>
+      </c>
+      <c r="O35" s="5">
+        <f t="shared" si="1"/>
+        <v>3.0585709999999999E-2</v>
+      </c>
+      <c r="P35" s="5">
+        <f t="shared" si="1"/>
+        <v>1.7063689999999999E-2</v>
+      </c>
+      <c r="Q35" s="5">
+        <f t="shared" si="1"/>
+        <v>1.7928880000000001E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>0.05</v>
       </c>
@@ -10098,8 +10369,56 @@
       <c r="C36">
         <v>1.7928880000000001E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F36" s="4">
+        <f t="shared" si="2"/>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G36" s="5">
+        <f t="shared" si="3"/>
+        <v>1.1566300000000001E-3</v>
+      </c>
+      <c r="H36" s="5">
+        <f t="shared" si="1"/>
+        <v>1.9855599999999999E-3</v>
+      </c>
+      <c r="I36" s="5">
+        <f t="shared" si="1"/>
+        <v>2.7274500000000002E-3</v>
+      </c>
+      <c r="J36" s="5">
+        <f t="shared" si="1"/>
+        <v>6.8210700000000003E-3</v>
+      </c>
+      <c r="K36" s="5">
+        <f t="shared" si="1"/>
+        <v>9.5325700000000006E-3</v>
+      </c>
+      <c r="L36" s="5">
+        <f t="shared" si="1"/>
+        <v>7.1575299999999996E-3</v>
+      </c>
+      <c r="M36" s="5">
+        <f t="shared" si="1"/>
+        <v>1.3089959999999999E-2</v>
+      </c>
+      <c r="N36" s="5">
+        <f t="shared" si="1"/>
+        <v>1.3966589999999999E-2</v>
+      </c>
+      <c r="O36" s="5">
+        <f t="shared" si="1"/>
+        <v>1.834479E-2</v>
+      </c>
+      <c r="P36" s="5">
+        <f t="shared" si="1"/>
+        <v>1.8071759999999999E-2</v>
+      </c>
+      <c r="Q36" s="5">
+        <f t="shared" si="1"/>
+        <v>1.6574519999999999E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -10109,8 +10428,56 @@
       <c r="C37">
         <v>1.1566300000000001E-3</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F37" s="4">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="G37" s="5">
+        <f t="shared" si="3"/>
+        <v>5.1018499999999998E-3</v>
+      </c>
+      <c r="H37" s="5">
+        <f t="shared" si="1"/>
+        <v>7.2120200000000004E-3</v>
+      </c>
+      <c r="I37" s="5">
+        <f t="shared" si="1"/>
+        <v>7.2126200000000003E-3</v>
+      </c>
+      <c r="J37" s="5">
+        <f t="shared" si="1"/>
+        <v>1.252114E-2</v>
+      </c>
+      <c r="K37" s="5">
+        <f t="shared" si="1"/>
+        <v>9.6894800000000003E-3</v>
+      </c>
+      <c r="L37" s="5">
+        <f t="shared" si="1"/>
+        <v>1.635853E-2</v>
+      </c>
+      <c r="M37" s="5">
+        <f t="shared" si="1"/>
+        <v>1.9624969999999999E-2</v>
+      </c>
+      <c r="N37" s="5">
+        <f t="shared" si="1"/>
+        <v>1.4778700000000001E-2</v>
+      </c>
+      <c r="O37" s="5">
+        <f t="shared" si="1"/>
+        <v>1.8468869999999998E-2</v>
+      </c>
+      <c r="P37" s="5">
+        <f t="shared" si="1"/>
+        <v>1.925321E-2</v>
+      </c>
+      <c r="Q37" s="5">
+        <f t="shared" si="1"/>
+        <v>1.8333240000000001E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -10120,8 +10487,56 @@
       <c r="C38">
         <v>1.9855599999999999E-3</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F38" s="4">
+        <f t="shared" si="2"/>
+        <v>0.125</v>
+      </c>
+      <c r="G38" s="5">
+        <f t="shared" si="3"/>
+        <v>1.1242299999999999E-3</v>
+      </c>
+      <c r="H38" s="5">
+        <f t="shared" si="1"/>
+        <v>3.0126200000000001E-3</v>
+      </c>
+      <c r="I38" s="5">
+        <f t="shared" si="1"/>
+        <v>1.8660659999999999E-2</v>
+      </c>
+      <c r="J38" s="5">
+        <f t="shared" si="1"/>
+        <v>1.148099E-2</v>
+      </c>
+      <c r="K38" s="5">
+        <f t="shared" si="1"/>
+        <v>9.0989199999999999E-3</v>
+      </c>
+      <c r="L38" s="5">
+        <f t="shared" si="1"/>
+        <v>1.795393E-2</v>
+      </c>
+      <c r="M38" s="5">
+        <f t="shared" si="1"/>
+        <v>1.7519730000000001E-2</v>
+      </c>
+      <c r="N38" s="5">
+        <f t="shared" si="1"/>
+        <v>1.7800219999999999E-2</v>
+      </c>
+      <c r="O38" s="5">
+        <f t="shared" si="1"/>
+        <v>1.8350760000000001E-2</v>
+      </c>
+      <c r="P38" s="5">
+        <f t="shared" si="1"/>
+        <v>1.7650869999999999E-2</v>
+      </c>
+      <c r="Q38" s="5">
+        <f t="shared" si="1"/>
+        <v>1.7375069999999999E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -10131,8 +10546,56 @@
       <c r="C39">
         <v>2.7274500000000002E-3</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F39" s="4">
+        <f t="shared" si="2"/>
+        <v>0.15</v>
+      </c>
+      <c r="G39" s="5">
+        <f t="shared" si="3"/>
+        <v>6.3868099999999997E-3</v>
+      </c>
+      <c r="H39" s="5">
+        <f t="shared" si="1"/>
+        <v>8.7306499999999995E-3</v>
+      </c>
+      <c r="I39" s="5">
+        <f t="shared" si="1"/>
+        <v>1.7362619999999999E-2</v>
+      </c>
+      <c r="J39" s="5">
+        <f t="shared" si="1"/>
+        <v>8.9120499999999995E-3</v>
+      </c>
+      <c r="K39" s="5">
+        <f t="shared" si="1"/>
+        <v>1.8993860000000001E-2</v>
+      </c>
+      <c r="L39" s="5">
+        <f t="shared" si="1"/>
+        <v>1.7674189999999999E-2</v>
+      </c>
+      <c r="M39" s="5">
+        <f t="shared" si="1"/>
+        <v>1.6555839999999999E-2</v>
+      </c>
+      <c r="N39" s="5">
+        <f t="shared" si="1"/>
+        <v>1.735915E-2</v>
+      </c>
+      <c r="O39" s="5">
+        <f t="shared" si="1"/>
+        <v>1.765806E-2</v>
+      </c>
+      <c r="P39" s="5">
+        <f t="shared" si="1"/>
+        <v>1.7935799999999998E-2</v>
+      </c>
+      <c r="Q39" s="5">
+        <f t="shared" si="1"/>
+        <v>1.8479639999999999E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -10142,8 +10605,56 @@
       <c r="C40">
         <v>6.8210700000000003E-3</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F40" s="4">
+        <f t="shared" si="2"/>
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="G40" s="5">
+        <f t="shared" si="3"/>
+        <v>1.483686E-2</v>
+      </c>
+      <c r="H40" s="5">
+        <f t="shared" si="1"/>
+        <v>1.84437E-2</v>
+      </c>
+      <c r="I40" s="5">
+        <f t="shared" si="1"/>
+        <v>7.4203699999999999E-3</v>
+      </c>
+      <c r="J40" s="5">
+        <f t="shared" si="1"/>
+        <v>1.903591E-2</v>
+      </c>
+      <c r="K40" s="5">
+        <f t="shared" si="1"/>
+        <v>1.792084E-2</v>
+      </c>
+      <c r="L40" s="5">
+        <f t="shared" si="1"/>
+        <v>1.2921810000000001E-2</v>
+      </c>
+      <c r="M40" s="5">
+        <f t="shared" si="1"/>
+        <v>1.8134790000000001E-2</v>
+      </c>
+      <c r="N40" s="5">
+        <f t="shared" si="1"/>
+        <v>1.7376800000000001E-2</v>
+      </c>
+      <c r="O40" s="5">
+        <f t="shared" si="1"/>
+        <v>1.6036789999999999E-2</v>
+      </c>
+      <c r="P40" s="5">
+        <f t="shared" si="1"/>
+        <v>1.8805820000000001E-2</v>
+      </c>
+      <c r="Q40" s="5">
+        <f t="shared" si="1"/>
+        <v>1.7925E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -10153,8 +10664,56 @@
       <c r="C41">
         <v>9.5325700000000006E-3</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F41" s="4">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="G41" s="5">
+        <f t="shared" si="3"/>
+        <v>5.3893099999999996E-3</v>
+      </c>
+      <c r="H41" s="5">
+        <f t="shared" si="1"/>
+        <v>9.2786099999999996E-3</v>
+      </c>
+      <c r="I41" s="5">
+        <f t="shared" si="1"/>
+        <v>7.8565500000000003E-3</v>
+      </c>
+      <c r="J41" s="5">
+        <f t="shared" si="1"/>
+        <v>1.8592609999999999E-2</v>
+      </c>
+      <c r="K41" s="5">
+        <f t="shared" si="1"/>
+        <v>1.686901E-2</v>
+      </c>
+      <c r="L41" s="5">
+        <f t="shared" si="1"/>
+        <v>1.707929E-2</v>
+      </c>
+      <c r="M41" s="5">
+        <f t="shared" si="1"/>
+        <v>1.6816149999999998E-2</v>
+      </c>
+      <c r="N41" s="5">
+        <f t="shared" si="1"/>
+        <v>1.8137469999999999E-2</v>
+      </c>
+      <c r="O41" s="5">
+        <f t="shared" si="1"/>
+        <v>1.9617699999999998E-2</v>
+      </c>
+      <c r="P41" s="5">
+        <f t="shared" si="1"/>
+        <v>1.9528340000000002E-2</v>
+      </c>
+      <c r="Q41" s="5">
+        <f t="shared" si="1"/>
+        <v>2.0015350000000001E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -10164,8 +10723,56 @@
       <c r="C42">
         <v>7.1575299999999996E-3</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F42" s="4">
+        <f t="shared" si="2"/>
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="G42" s="5">
+        <f t="shared" si="3"/>
+        <v>7.7603699999999999E-3</v>
+      </c>
+      <c r="H42" s="5">
+        <f t="shared" si="1"/>
+        <v>1.715937E-2</v>
+      </c>
+      <c r="I42" s="5">
+        <f t="shared" si="1"/>
+        <v>1.759904E-2</v>
+      </c>
+      <c r="J42" s="5">
+        <f t="shared" si="1"/>
+        <v>1.7165779999999999E-2</v>
+      </c>
+      <c r="K42" s="5">
+        <f t="shared" si="1"/>
+        <v>1.734552E-2</v>
+      </c>
+      <c r="L42" s="5">
+        <f t="shared" si="1"/>
+        <v>1.7712229999999999E-2</v>
+      </c>
+      <c r="M42" s="5">
+        <f t="shared" si="1"/>
+        <v>1.886612E-2</v>
+      </c>
+      <c r="N42" s="5">
+        <f t="shared" si="1"/>
+        <v>1.6565739999999999E-2</v>
+      </c>
+      <c r="O42" s="5">
+        <f t="shared" si="1"/>
+        <v>1.800146E-2</v>
+      </c>
+      <c r="P42" s="5">
+        <f t="shared" si="1"/>
+        <v>1.9145120000000002E-2</v>
+      </c>
+      <c r="Q42" s="5">
+        <f t="shared" si="1"/>
+        <v>1.932149E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -10175,8 +10782,56 @@
       <c r="C43">
         <v>1.3089959999999999E-2</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F43" s="4">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="G43" s="5">
+        <f t="shared" si="3"/>
+        <v>2.1218290000000001E-2</v>
+      </c>
+      <c r="H43" s="5">
+        <f t="shared" si="1"/>
+        <v>1.5721329999999999E-2</v>
+      </c>
+      <c r="I43" s="5">
+        <f t="shared" si="1"/>
+        <v>1.7473760000000001E-2</v>
+      </c>
+      <c r="J43" s="5">
+        <f t="shared" si="1"/>
+        <v>1.749674E-2</v>
+      </c>
+      <c r="K43" s="5">
+        <f t="shared" si="1"/>
+        <v>2.2159120000000001E-2</v>
+      </c>
+      <c r="L43" s="5">
+        <f t="shared" si="1"/>
+        <v>1.6790920000000001E-2</v>
+      </c>
+      <c r="M43" s="5">
+        <f t="shared" si="1"/>
+        <v>1.9198920000000001E-2</v>
+      </c>
+      <c r="N43" s="5">
+        <f t="shared" si="1"/>
+        <v>1.8518960000000001E-2</v>
+      </c>
+      <c r="O43" s="5">
+        <f t="shared" si="1"/>
+        <v>1.914482E-2</v>
+      </c>
+      <c r="P43" s="5">
+        <f t="shared" si="1"/>
+        <v>1.9505339999999999E-2</v>
+      </c>
+      <c r="Q43" s="5">
+        <f t="shared" si="1"/>
+        <v>2.326611E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -10187,7 +10842,7 @@
         <v>1.3966589999999999E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -10198,7 +10853,7 @@
         <v>1.834479E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -10209,7 +10864,7 @@
         <v>1.8071759999999999E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -10220,7 +10875,7 @@
         <v>1.6574519999999999E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>0.1</v>
       </c>
@@ -11080,7 +11735,74 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="G33:Q42">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="2.5000000000000001E-2"/>
+        <color theme="3" tint="0.39997558519241921"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{0F09356E-91FC-401C-B141-FEA226CBB906}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G43:Q43">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="2.5000000000000001E-2"/>
+        <color theme="3" tint="0.39997558519241921"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{0F0BECC1-BB39-4E4B-BB24-74660EC66633}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="G32:Q32" formulaRange="1"/>
+  </ignoredErrors>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{0F09356E-91FC-401C-B141-FEA226CBB906}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2.5000000000000001E-2</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G33:Q42</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{0F0BECC1-BB39-4E4B-BB24-74660EC66633}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2.5000000000000001E-2</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G43:Q43</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modify: compare 10 smallest values for each algorithm
</commit_message>
<xml_diff>
--- a/2020_01_32770/Result.xlsx
+++ b/2020_01_32770/Result.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Random Search</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -65,15 +65,21 @@
     <t>lr/dropout</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>SMALL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="0.000000_);[Red]\(0.000000\)"/>
+  <numFmts count="3">
+    <numFmt numFmtId="176" formatCode="0.000000_);[Red]\(0.000000\)"/>
+    <numFmt numFmtId="177" formatCode="0.000000_ "/>
+    <numFmt numFmtId="178" formatCode="0.0000_ "/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +101,14 @@
       <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3" tint="0.39997558519241921"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
@@ -148,7 +162,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -158,13 +172,28 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -199,7 +228,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7773,7 +7801,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E30" workbookViewId="0">
+      <selection activeCell="K49" sqref="K49"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
@@ -8122,7 +8152,7 @@
         <v>0</v>
       </c>
       <c r="H32" s="4">
-        <f t="shared" ref="H32:R32" si="0">INDEX($B4:$B14, COLUMN()-6)</f>
+        <f t="shared" ref="H32:Q32" si="0">INDEX($B4:$B14, COLUMN()-6)</f>
         <v>2.354494E-2</v>
       </c>
       <c r="I32" s="4">
@@ -8236,7 +8266,7 @@
         <v>6.1594099999999997E-3</v>
       </c>
       <c r="G34" s="5">
-        <f t="shared" ref="G34:Q43" si="3">INDEX($C$4:$C$124, (ROW()-33)*11+(COLUMN()-7)+1)</f>
+        <f t="shared" ref="G34:G43" si="3">INDEX($C$4:$C$124, (ROW()-33)*11+(COLUMN()-7)+1)</f>
         <v>1.0613E-4</v>
       </c>
       <c r="H34" s="5">
@@ -8832,6 +8862,10 @@
       <c r="C45">
         <v>1.8657599999999999E-3</v>
       </c>
+      <c r="F45" s="7"/>
+      <c r="G45" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A46">
@@ -8843,6 +8877,20 @@
       <c r="C46">
         <v>2.3009800000000002E-3</v>
       </c>
+      <c r="F46" s="6">
+        <v>1</v>
+      </c>
+      <c r="G46" s="8">
+        <f>SMALL($G$33:$Q$43, F46)</f>
+        <v>5.6919999999999997E-5</v>
+      </c>
+      <c r="H46" s="9">
+        <v>1.2011E-4</v>
+      </c>
+      <c r="I46" s="10">
+        <f>H46/G46</f>
+        <v>2.110154602951511</v>
+      </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A47">
@@ -8854,6 +8902,20 @@
       <c r="C47">
         <v>9.9460299999999998E-3</v>
       </c>
+      <c r="F47" s="6">
+        <v>2</v>
+      </c>
+      <c r="G47" s="8">
+        <f t="shared" ref="G47:G55" si="5">SMALL($G$33:$Q$43, F47)</f>
+        <v>7.6100000000000007E-5</v>
+      </c>
+      <c r="H47" s="9">
+        <v>1.4980000000000001E-4</v>
+      </c>
+      <c r="I47" s="10">
+        <f t="shared" ref="I47:I55" si="6">H47/G47</f>
+        <v>1.9684625492772667</v>
+      </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A48">
@@ -8865,8 +8927,22 @@
       <c r="C48">
         <v>1.3789999999999999E-4</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F48" s="6">
+        <v>3</v>
+      </c>
+      <c r="G48" s="8">
+        <f t="shared" si="5"/>
+        <v>8.6500000000000002E-5</v>
+      </c>
+      <c r="H48" s="9">
+        <v>1.1242299999999999E-3</v>
+      </c>
+      <c r="I48" s="10">
+        <f t="shared" si="6"/>
+        <v>12.996878612716761</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>2.4637639999999999E-2</v>
       </c>
@@ -8876,8 +8952,22 @@
       <c r="C49">
         <v>2.2132E-4</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F49" s="6">
+        <v>4</v>
+      </c>
+      <c r="G49" s="8">
+        <f t="shared" si="5"/>
+        <v>9.6899999999999997E-5</v>
+      </c>
+      <c r="H49" s="9">
+        <v>1.1566300000000001E-3</v>
+      </c>
+      <c r="I49" s="10">
+        <f t="shared" si="6"/>
+        <v>11.936326109391127</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>2.4637639999999999E-2</v>
       </c>
@@ -8887,8 +8977,22 @@
       <c r="C50">
         <v>5.2793000000000002E-4</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F50" s="6">
+        <v>5</v>
+      </c>
+      <c r="G50" s="8">
+        <f t="shared" si="5"/>
+        <v>1.0016E-4</v>
+      </c>
+      <c r="H50" s="9">
+        <v>1.18139E-3</v>
+      </c>
+      <c r="I50" s="10">
+        <f t="shared" si="6"/>
+        <v>11.795027955271566</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51">
         <v>2.4637639999999999E-2</v>
       </c>
@@ -8898,8 +9002,22 @@
       <c r="C51">
         <v>8.3421000000000005E-4</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F51" s="6">
+        <v>6</v>
+      </c>
+      <c r="G51" s="8">
+        <f t="shared" si="5"/>
+        <v>1.0613E-4</v>
+      </c>
+      <c r="H51" s="9">
+        <v>1.7269399999999999E-3</v>
+      </c>
+      <c r="I51" s="10">
+        <f t="shared" si="6"/>
+        <v>16.271930651088287</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52">
         <v>2.4637639999999999E-2</v>
       </c>
@@ -8909,8 +9027,22 @@
       <c r="C52">
         <v>1.5403299999999999E-3</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F52" s="6">
+        <v>7</v>
+      </c>
+      <c r="G52" s="8">
+        <f t="shared" si="5"/>
+        <v>1.3789999999999999E-4</v>
+      </c>
+      <c r="H52" s="9">
+        <v>1.9855599999999999E-3</v>
+      </c>
+      <c r="I52" s="10">
+        <f t="shared" si="6"/>
+        <v>14.398549673676577</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>2.4637639999999999E-2</v>
       </c>
@@ -8920,8 +9052,22 @@
       <c r="C53">
         <v>5.66732E-3</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F53" s="6">
+        <v>8</v>
+      </c>
+      <c r="G53" s="8">
+        <f t="shared" si="5"/>
+        <v>1.4370999999999999E-4</v>
+      </c>
+      <c r="H53" s="9">
+        <v>2.0390199999999999E-3</v>
+      </c>
+      <c r="I53" s="10">
+        <f t="shared" si="6"/>
+        <v>14.188435042794517</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>2.4637639999999999E-2</v>
       </c>
@@ -8931,8 +9077,22 @@
       <c r="C54">
         <v>1.18333E-3</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F54" s="6">
+        <v>9</v>
+      </c>
+      <c r="G54" s="8">
+        <f t="shared" si="5"/>
+        <v>2.1043E-4</v>
+      </c>
+      <c r="H54" s="9">
+        <v>2.7274500000000002E-3</v>
+      </c>
+      <c r="I54" s="10">
+        <f t="shared" si="6"/>
+        <v>12.96131730266597</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>2.4637639999999999E-2</v>
       </c>
@@ -8942,8 +9102,22 @@
       <c r="C55">
         <v>3.1705499999999998E-3</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F55" s="6">
+        <v>10</v>
+      </c>
+      <c r="G55" s="8">
+        <f t="shared" si="5"/>
+        <v>2.2132E-4</v>
+      </c>
+      <c r="H55" s="9">
+        <v>2.8408299999999999E-3</v>
+      </c>
+      <c r="I55" s="10">
+        <f t="shared" si="6"/>
+        <v>12.835848545093077</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>2.4637639999999999E-2</v>
       </c>
@@ -8954,7 +9128,7 @@
         <v>4.45437E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>2.4637639999999999E-2</v>
       </c>
@@ -8965,7 +9139,7 @@
         <v>3.6485799999999998E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>2.4637639999999999E-2</v>
       </c>
@@ -8976,7 +9150,7 @@
         <v>5.54522E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>3.0797060000000001E-2</v>
       </c>
@@ -8987,7 +9161,7 @@
         <v>8.6500000000000002E-5</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A60">
         <v>3.0797060000000001E-2</v>
       </c>
@@ -8998,7 +9172,7 @@
         <v>5.8699999999999996E-4</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>3.0797060000000001E-2</v>
       </c>
@@ -9009,7 +9183,7 @@
         <v>5.4730000000000002E-4</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A62">
         <v>3.0797060000000001E-2</v>
       </c>
@@ -9020,7 +9194,7 @@
         <v>3.1371699999999999E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A63">
         <v>3.0797060000000001E-2</v>
       </c>
@@ -9031,7 +9205,7 @@
         <v>1.4363799999999999E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A64">
         <v>3.0797060000000001E-2</v>
       </c>
@@ -9792,8 +9966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q125"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46:G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -10256,7 +10430,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="G34" s="5">
-        <f t="shared" ref="G34:Q43" si="3">INDEX($C$4:$C$124, (ROW()-33)*11+(COLUMN()-7)+1)</f>
+        <f t="shared" ref="G34:G43" si="3">INDEX($C$4:$C$124, (ROW()-33)*11+(COLUMN()-7)+1)</f>
         <v>1.2011E-4</v>
       </c>
       <c r="H34" s="5">
@@ -10852,6 +11026,10 @@
       <c r="C45">
         <v>1.834479E-2</v>
       </c>
+      <c r="F45" s="7"/>
+      <c r="G45" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A46">
@@ -10863,6 +11041,13 @@
       <c r="C46">
         <v>1.8071759999999999E-2</v>
       </c>
+      <c r="F46" s="6">
+        <v>1</v>
+      </c>
+      <c r="G46" s="8">
+        <f>SMALL($G$33:$Q$43, F46)</f>
+        <v>1.2011E-4</v>
+      </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A47">
@@ -10874,6 +11059,13 @@
       <c r="C47">
         <v>1.6574519999999999E-2</v>
       </c>
+      <c r="F47" s="6">
+        <v>2</v>
+      </c>
+      <c r="G47" s="8">
+        <f t="shared" ref="G47:G55" si="4">SMALL($G$33:$Q$43, F47)</f>
+        <v>1.4980000000000001E-4</v>
+      </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A48">
@@ -10885,8 +11077,15 @@
       <c r="C48">
         <v>5.1018499999999998E-3</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F48" s="6">
+        <v>3</v>
+      </c>
+      <c r="G48" s="8">
+        <f t="shared" si="4"/>
+        <v>1.1242299999999999E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>0.1</v>
       </c>
@@ -10896,8 +11095,15 @@
       <c r="C49">
         <v>7.2120200000000004E-3</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F49" s="6">
+        <v>4</v>
+      </c>
+      <c r="G49" s="8">
+        <f t="shared" si="4"/>
+        <v>1.1566300000000001E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>0.1</v>
       </c>
@@ -10907,8 +11113,15 @@
       <c r="C50">
         <v>7.2126200000000003E-3</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F50" s="6">
+        <v>5</v>
+      </c>
+      <c r="G50" s="8">
+        <f t="shared" si="4"/>
+        <v>1.18139E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51">
         <v>0.1</v>
       </c>
@@ -10918,8 +11131,15 @@
       <c r="C51">
         <v>1.252114E-2</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F51" s="6">
+        <v>6</v>
+      </c>
+      <c r="G51" s="8">
+        <f t="shared" si="4"/>
+        <v>1.7269399999999999E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A52">
         <v>0.1</v>
       </c>
@@ -10929,8 +11149,15 @@
       <c r="C52">
         <v>9.6894800000000003E-3</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F52" s="6">
+        <v>7</v>
+      </c>
+      <c r="G52" s="8">
+        <f t="shared" si="4"/>
+        <v>1.9855599999999999E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>0.1</v>
       </c>
@@ -10940,8 +11167,15 @@
       <c r="C53">
         <v>1.635853E-2</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F53" s="6">
+        <v>8</v>
+      </c>
+      <c r="G53" s="8">
+        <f t="shared" si="4"/>
+        <v>2.0390199999999999E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>0.1</v>
       </c>
@@ -10951,8 +11185,15 @@
       <c r="C54">
         <v>1.9624969999999999E-2</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F54" s="6">
+        <v>9</v>
+      </c>
+      <c r="G54" s="8">
+        <f t="shared" si="4"/>
+        <v>2.7274500000000002E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>0.1</v>
       </c>
@@ -10962,8 +11203,15 @@
       <c r="C55">
         <v>1.4778700000000001E-2</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F55" s="6">
+        <v>10</v>
+      </c>
+      <c r="G55" s="8">
+        <f t="shared" si="4"/>
+        <v>2.8408299999999999E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>0.1</v>
       </c>
@@ -10974,7 +11222,7 @@
         <v>1.8468869999999998E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>0.1</v>
       </c>
@@ -10985,7 +11233,7 @@
         <v>1.925321E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>0.1</v>
       </c>
@@ -10996,7 +11244,7 @@
         <v>1.8333240000000001E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>0.125</v>
       </c>
@@ -11007,7 +11255,7 @@
         <v>1.1242299999999999E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60">
         <v>0.125</v>
       </c>
@@ -11018,7 +11266,7 @@
         <v>3.0126200000000001E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>0.125</v>
       </c>
@@ -11029,7 +11277,7 @@
         <v>1.8660659999999999E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62">
         <v>0.125</v>
       </c>
@@ -11040,7 +11288,7 @@
         <v>1.148099E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63">
         <v>0.125</v>
       </c>
@@ -11051,7 +11299,7 @@
         <v>9.0989199999999999E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64">
         <v>0.125</v>
       </c>

</xml_diff>